<commit_message>
Suite Module and Doc Pro New UI Change fixes
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Omnex\Repo\OmnexAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0682F9D0-EEB1-46AF-A865-A16B4AD9C8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557D3BE9-1E32-421D-8C44-470082047889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -659,7 +659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,6 +699,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -900,59 +906,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B084"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3306,7 +3272,7 @@
   <dimension ref="A1:AN15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3464,10 +3430,10 @@
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A2" s="25">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3516,10 +3482,10 @@
       <c r="AN2" s="12"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>156</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -3578,10 +3544,10 @@
       <c r="AN3" s="12"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>163</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3650,10 +3616,10 @@
       <c r="AN4" s="12"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -3718,10 +3684,10 @@
       <c r="AN5" s="12"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>169</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -3790,10 +3756,10 @@
       <c r="AN6" s="12"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>170</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -3860,10 +3826,10 @@
       <c r="AN7" s="12"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A8" s="25">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>175</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -3924,10 +3890,10 @@
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A9" s="25">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>159</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -3986,10 +3952,10 @@
       <c r="AN9" s="12"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A10" s="25">
+      <c r="A10" s="24">
         <v>9</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>172</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -4060,10 +4026,10 @@
       <c r="AN10" s="12"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A11" s="25">
+      <c r="A11" s="24">
         <v>10</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>173</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -4134,10 +4100,10 @@
       <c r="AN11" s="12"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A12" s="25">
+      <c r="A12" s="24">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>121</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -4188,10 +4154,10 @@
       <c r="AN12" s="12"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A13" s="25">
+      <c r="A13" s="24">
         <v>12</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="25" t="s">
         <v>124</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4262,10 +4228,10 @@
       <c r="AN13" s="12"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A14" s="25">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="25" t="s">
         <v>143</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -4329,11 +4295,11 @@
       <c r="AM14" s="12"/>
       <c r="AN14" s="12"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A15" s="25">
+    <row r="15" spans="1:40" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="24">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -4384,7 +4350,7 @@
   </sheetData>
   <autoFilter ref="A1:AN1" xr:uid="{E894568B-9590-425D-B70B-CA0CE93C4D0E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN15">
-      <sortCondition sortBy="cellColor" ref="B1" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="B1" dxfId="0"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>